<commit_message>
Add source code file paths, clean up charts
</commit_message>
<xml_diff>
--- a/powerflowpy/tests/timings/dss_detailed_timing.xlsx
+++ b/powerflowpy/tests/timings/dss_detailed_timing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elainelaguerta/Dropbox/LBNL/LinDist3Flow/powerflowpy/tests/timings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C67EB12-D46E-F542-B661-A3A39914B6D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18272C-A713-454F-BF86-D6A55E91B6D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dss_detailed_timing_data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>total_time</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>num_iterations</t>
+  </si>
+  <si>
+    <t>Source code filepath: LinDistFlow/powerflowpy/powerflowpy/dss_solve_detailed_timing.py</t>
+  </si>
+  <si>
+    <t>Source code: LinDist3Flow/powerflowpy/dss_timer.py</t>
   </si>
 </sst>
 </file>
@@ -667,11 +673,771 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="5"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>dss_detailed_timing_data!$C$2</c:f>
+              <c:f>dss_detailed_timing_data!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>reset_loads_total_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14569653674384639"/>
+                  <c:y val="9.9303234577692166E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dss_detailed_timing_data!$E$4:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>14.4324469999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.6166410000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.101370000000998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.031578000000302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.480816000000502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.957272000002106</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105.927956000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.62099800000101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160.90479500000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>195.29794099999501</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>164.91186099999001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>177.45008699999701</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180.60015900000101</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>191.84692499999599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>217.59380299999299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>229.60053099999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>234.242576000009</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>297.87461099999302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>262.18401799999799</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>326.13471199999202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-9DCC-F74F-A016-282964A0E918}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dss_detailed_timing_data!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>save_loads_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15520902188058835"/>
+                  <c:y val="-4.1115957627598709E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dss_detailed_timing_data!$D$4:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.7895059999999399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8133059999999599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.993594000000099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.418425999999901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.7969919999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.827808000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32.489599999999797</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.055908000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46.742635000000199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65.605849000000205</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.943229999999303</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.508581000000397</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.072312000000601</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59.224690000000997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>68.974967999999507</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>72.330826999999502</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>70.088992999998396</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.852418999998704</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>81.400444999998996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>88.396274999999093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-9DCC-F74F-A016-282964A0E918}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dss_detailed_timing_data!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>final_calcs_time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15283090059640295"/>
+                  <c:y val="-6.7499008667082083E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dss_detailed_timing_data!$G$4:$G$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2.2577189999999301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2084469999998904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3967719999998804</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.52736300000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.544297</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.674081999999601</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.968339000000299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.527332000000101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.638249000000201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.730349999999898</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.538242000000199</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.500899000000398</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.383750000000799</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.8098660000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32.707938999998397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33.508222000000899</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>33.467724000001603</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47.126156999999203</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.163927999999103</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.654012000000101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-9DCC-F74F-A016-282964A0E918}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dss_detailed_timing_data!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -774,7 +1540,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$3:$A$22</c:f>
+              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -843,7 +1609,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>dss_detailed_timing_data!$C$3:$C$22</c:f>
+              <c:f>dss_detailed_timing_data!$C$4:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -918,513 +1684,11 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
+          <c:idx val="6"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>dss_detailed_timing_data!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>save_loads_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent5">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.15520902188058835"/>
-                  <c:y val="-4.1115957627598709E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$3:$A$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$D$3:$D$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>4.7895059999999399</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8133059999999599</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.993594000000099</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.418425999999901</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.7969919999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24.827808000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32.489599999999797</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>46.055908000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>46.742635000000199</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65.605849000000205</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49.943229999999303</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>49.508581000000397</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>58.072312000000601</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>59.224690000000997</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>68.974967999999507</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>72.330826999999502</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>70.088992999998396</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>89.852418999998704</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>81.400444999998996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>88.396274999999093</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-9DCC-F74F-A016-282964A0E918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>dss_detailed_timing_data!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>reset_loads_total_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.14569653674384639"/>
-                  <c:y val="9.9303234577692166E-4"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$3:$A$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$E$3:$E$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>14.4324469999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28.6166410000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.101370000000998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55.031578000000302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>71.480816000000502</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>82.957272000002106</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105.927956000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>140.62099800000101</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>160.90479500000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>195.29794099999501</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>164.91186099999001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>177.45008699999701</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>180.60015900000101</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>191.84692499999599</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>217.59380299999299</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>229.60053099999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>234.242576000009</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>297.87461099999302</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>262.18401799999799</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>326.13471199999202</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-9DCC-F74F-A016-282964A0E918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>dss_detailed_timing_data!$F$2</c:f>
+              <c:f>dss_detailed_timing_data!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1534,7 +1798,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$3:$A$22</c:f>
+              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1603,7 +1867,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>dss_detailed_timing_data!$F$3:$F$22</c:f>
+              <c:f>dss_detailed_timing_data!$F$4:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1674,264 +1938,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-9DCC-F74F-A016-282964A0E918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>dss_detailed_timing_data!$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>final_calcs_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.15283090059640295"/>
-                  <c:y val="-6.7499008667082083E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$3:$A$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$G$3:$G$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>2.2577189999999301</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.2084469999998904</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.3967719999998804</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.52736300000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.544297</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.674081999999601</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.968339000000299</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>22.527332000000101</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>23.638249000000201</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>31.730349999999898</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>24.538242000000199</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>28.500899000000398</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26.383750000000799</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>27.8098660000005</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32.707938999998397</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>33.508222000000899</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>33.467724000001603</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>47.126156999999203</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>37.163927999999103</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43.654012000000101</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-9DCC-F74F-A016-282964A0E918}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2173,6 +2179,26 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -2180,7 +2206,7 @@
           <c:x val="0.78133942531856526"/>
           <c:y val="0.29795207613436808"/>
           <c:w val="0.21271527147097097"/>
-          <c:h val="0.38351951509658416"/>
+          <c:h val="0.2324403784059367"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2803,19 +2829,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>init_circuit_time</c:v>
+                  <c:v>reset_loads_total_time</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>save_loads_time</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>reset_loads_total_time</c:v>
+                  <c:v>final_calcs_time</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>init_circuit_time</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>run_solvesnap_total_time</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>final_calcs_time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2827,19 +2853,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.6125</c:v>
+                  <c:v>14.898999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.4188999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.898999999999999</c:v>
+                  <c:v>2.1086</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.6125</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.0423</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.1086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4227,13 +4253,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>164519</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>111571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4257,7 +4283,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="0" y="406400"/>
           <a:ext cx="12547019" cy="28965971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4567,499 +4593,502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
         <v>1</v>
-      </c>
-      <c r="B3">
-        <v>23.4771069999994</v>
-      </c>
-      <c r="C3">
-        <v>1.039534</v>
-      </c>
-      <c r="D3">
-        <v>4.7895059999999399</v>
-      </c>
-      <c r="E3">
-        <v>14.4324469999997</v>
-      </c>
-      <c r="F3">
-        <v>0.95790099999981604</v>
-      </c>
-      <c r="G3">
-        <v>2.2577189999999301</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>46.656638999999899</v>
+        <v>23.4771069999994</v>
       </c>
       <c r="C4">
-        <v>2.9911470000000202</v>
+        <v>1.039534</v>
       </c>
       <c r="D4">
-        <v>8.8133059999999599</v>
+        <v>4.7895059999999399</v>
       </c>
       <c r="E4">
-        <v>28.6166410000003</v>
+        <v>14.4324469999997</v>
       </c>
       <c r="F4">
-        <v>2.0270979999996701</v>
+        <v>0.95790099999981604</v>
       </c>
       <c r="G4">
-        <v>4.2084469999998904</v>
+        <v>2.2577189999999301</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>69.815775999999602</v>
+        <v>46.656638999999899</v>
       </c>
       <c r="C5">
-        <v>4.4325089999999099</v>
+        <v>2.9911470000000202</v>
       </c>
       <c r="D5">
-        <v>12.993594000000099</v>
+        <v>8.8133059999999599</v>
       </c>
       <c r="E5">
-        <v>43.101370000000998</v>
+        <v>28.6166410000003</v>
       </c>
       <c r="F5">
-        <v>2.8915309999987202</v>
+        <v>2.0270979999996701</v>
       </c>
       <c r="G5">
-        <v>6.3967719999998804</v>
+        <v>4.2084469999998904</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>90.736822999999603</v>
+        <v>69.815775999999602</v>
       </c>
       <c r="C6">
-        <v>5.9425699999999804</v>
+        <v>4.4325089999999099</v>
       </c>
       <c r="D6">
-        <v>16.418425999999901</v>
+        <v>12.993594000000099</v>
       </c>
       <c r="E6">
-        <v>55.031578000000302</v>
+        <v>43.101370000000998</v>
       </c>
       <c r="F6">
-        <v>3.8168859999992901</v>
+        <v>2.8915309999987202</v>
       </c>
       <c r="G6">
-        <v>9.52736300000001</v>
+        <v>6.3967719999998804</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>115.293122999999</v>
+        <v>90.736822999999603</v>
       </c>
       <c r="C7">
-        <v>7.4880870000000304</v>
+        <v>5.9425699999999804</v>
       </c>
       <c r="D7">
-        <v>20.7969919999999</v>
+        <v>16.418425999999901</v>
       </c>
       <c r="E7">
-        <v>71.480816000000502</v>
+        <v>55.031578000000302</v>
       </c>
       <c r="F7">
-        <v>4.9829309999986897</v>
+        <v>3.8168859999992901</v>
       </c>
       <c r="G7">
-        <v>10.544297</v>
+        <v>9.52736300000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>135.48738599999899</v>
+        <v>115.293122999999</v>
       </c>
       <c r="C8">
-        <v>9.4209569999999996</v>
+        <v>7.4880870000000304</v>
       </c>
       <c r="D8">
-        <v>24.827808000000001</v>
+        <v>20.7969919999999</v>
       </c>
       <c r="E8">
-        <v>82.957272000002106</v>
+        <v>71.480816000000502</v>
       </c>
       <c r="F8">
-        <v>5.6072669999980196</v>
+        <v>4.9829309999986897</v>
       </c>
       <c r="G8">
-        <v>12.674081999999601</v>
+        <v>10.544297</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>174.798915999998</v>
+        <v>135.48738599999899</v>
       </c>
       <c r="C9">
-        <v>11.508993</v>
+        <v>9.4209569999999996</v>
       </c>
       <c r="D9">
-        <v>32.489599999999797</v>
+        <v>24.827808000000001</v>
       </c>
       <c r="E9">
-        <v>105.927956000001</v>
+        <v>82.957272000002106</v>
       </c>
       <c r="F9">
-        <v>7.9040279999964502</v>
+        <v>5.6072669999980196</v>
       </c>
       <c r="G9">
-        <v>16.968339000000299</v>
+        <v>12.674081999999601</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>234.42470699999899</v>
+        <v>174.798915999998</v>
       </c>
       <c r="C10">
-        <v>14.604229999999699</v>
+        <v>11.508993</v>
       </c>
       <c r="D10">
-        <v>46.055908000000002</v>
+        <v>32.489599999999797</v>
       </c>
       <c r="E10">
-        <v>140.62099800000101</v>
+        <v>105.927956000001</v>
       </c>
       <c r="F10">
-        <v>10.616238999997501</v>
+        <v>7.9040279999964502</v>
       </c>
       <c r="G10">
-        <v>22.527332000000101</v>
+        <v>16.968339000000299</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>262.62673900000198</v>
+        <v>234.42470699999899</v>
       </c>
       <c r="C11">
-        <v>15.4100939999999</v>
+        <v>14.604229999999699</v>
       </c>
       <c r="D11">
-        <v>46.742635000000199</v>
+        <v>46.055908000000002</v>
       </c>
       <c r="E11">
-        <v>160.90479500000001</v>
+        <v>140.62099800000101</v>
       </c>
       <c r="F11">
-        <v>15.9309660000013</v>
+        <v>10.616238999997501</v>
       </c>
       <c r="G11">
-        <v>23.638249000000201</v>
+        <v>22.527332000000101</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>334.14372200000003</v>
+        <v>262.62673900000198</v>
       </c>
       <c r="C12">
-        <v>22.569173999999801</v>
+        <v>15.4100939999999</v>
       </c>
       <c r="D12">
-        <v>65.605849000000205</v>
+        <v>46.742635000000199</v>
       </c>
       <c r="E12">
-        <v>195.29794099999501</v>
+        <v>160.90479500000001</v>
       </c>
       <c r="F12">
-        <v>18.940408000004801</v>
+        <v>15.9309660000013</v>
       </c>
       <c r="G12">
-        <v>31.730349999999898</v>
+        <v>23.638249000000201</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>269.24663100001197</v>
+        <v>334.14372200000003</v>
       </c>
       <c r="C13">
-        <v>17.957875999999999</v>
+        <v>22.569173999999801</v>
       </c>
       <c r="D13">
-        <v>49.943229999999303</v>
+        <v>65.605849000000205</v>
       </c>
       <c r="E13">
-        <v>164.91186099999001</v>
+        <v>195.29794099999501</v>
       </c>
       <c r="F13">
-        <v>11.895422000021499</v>
+        <v>18.940408000004801</v>
       </c>
       <c r="G13">
-        <v>24.538242000000199</v>
+        <v>31.730349999999898</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>290.40433199999302</v>
+        <v>269.24663100001197</v>
       </c>
       <c r="C14">
-        <v>21.995880000000401</v>
+        <v>17.957875999999999</v>
       </c>
       <c r="D14">
-        <v>49.508581000000397</v>
+        <v>49.943229999999303</v>
       </c>
       <c r="E14">
-        <v>177.45008699999701</v>
+        <v>164.91186099999001</v>
       </c>
       <c r="F14">
-        <v>12.9488849999943</v>
+        <v>11.895422000021499</v>
       </c>
       <c r="G14">
-        <v>28.500899000000398</v>
+        <v>24.538242000000199</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>297.15531299999401</v>
+        <v>290.40433199999302</v>
       </c>
       <c r="C15">
-        <v>19.676685999999499</v>
+        <v>21.995880000000401</v>
       </c>
       <c r="D15">
-        <v>58.072312000000601</v>
+        <v>49.508581000000397</v>
       </c>
       <c r="E15">
-        <v>180.60015900000101</v>
+        <v>177.45008699999701</v>
       </c>
       <c r="F15">
-        <v>12.422405999992201</v>
+        <v>12.9488849999943</v>
       </c>
       <c r="G15">
-        <v>26.383750000000799</v>
+        <v>28.500899000000398</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>314.076350999981</v>
+        <v>297.15531299999401</v>
       </c>
       <c r="C16">
-        <v>22.175610999998799</v>
+        <v>19.676685999999499</v>
       </c>
       <c r="D16">
-        <v>59.224690000000997</v>
+        <v>58.072312000000601</v>
       </c>
       <c r="E16">
-        <v>191.84692499999599</v>
+        <v>180.60015900000101</v>
       </c>
       <c r="F16">
-        <v>13.019258999984901</v>
+        <v>12.422405999992201</v>
       </c>
       <c r="G16">
-        <v>27.8098660000005</v>
+        <v>26.383750000000799</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>358.19276399999399</v>
+        <v>314.076350999981</v>
       </c>
       <c r="C17">
-        <v>23.917985999998901</v>
+        <v>22.175610999998799</v>
       </c>
       <c r="D17">
-        <v>68.974967999999507</v>
+        <v>59.224690000000997</v>
       </c>
       <c r="E17">
-        <v>217.59380299999299</v>
+        <v>191.84692499999599</v>
       </c>
       <c r="F17">
-        <v>14.9980680000041</v>
+        <v>13.019258999984901</v>
       </c>
       <c r="G17">
-        <v>32.707938999998397</v>
+        <v>27.8098660000005</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>376.30753899999502</v>
+        <v>358.19276399999399</v>
       </c>
       <c r="C18">
-        <v>24.7659270000002</v>
+        <v>23.917985999998901</v>
       </c>
       <c r="D18">
-        <v>72.330826999999502</v>
+        <v>68.974967999999507</v>
       </c>
       <c r="E18">
-        <v>229.60053099999999</v>
+        <v>217.59380299999299</v>
       </c>
       <c r="F18">
-        <v>16.1020319999942</v>
+        <v>14.9980680000041</v>
       </c>
       <c r="G18">
-        <v>33.508222000000899</v>
+        <v>32.707938999998397</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>379.55428800001198</v>
+        <v>376.30753899999502</v>
       </c>
       <c r="C19">
-        <v>25.994071999999498</v>
+        <v>24.7659270000002</v>
       </c>
       <c r="D19">
-        <v>70.088992999998396</v>
+        <v>72.330826999999502</v>
       </c>
       <c r="E19">
-        <v>234.242576000009</v>
+        <v>229.60053099999999</v>
       </c>
       <c r="F19">
-        <v>15.7609230000037</v>
+        <v>16.1020319999942</v>
       </c>
       <c r="G19">
-        <v>33.467724000001603</v>
+        <v>33.508222000000899</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>485.88818599998098</v>
+        <v>379.55428800001198</v>
       </c>
       <c r="C20">
-        <v>29.882386000000501</v>
+        <v>25.994071999999498</v>
       </c>
       <c r="D20">
-        <v>89.852418999998704</v>
+        <v>70.088992999998396</v>
       </c>
       <c r="E20">
-        <v>297.87461099999302</v>
+        <v>234.242576000009</v>
       </c>
       <c r="F20">
-        <v>21.152612999990101</v>
+        <v>15.7609230000037</v>
       </c>
       <c r="G20">
-        <v>47.126156999999203</v>
+        <v>33.467724000001603</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>428.77268199996701</v>
+        <v>485.88818599998098</v>
       </c>
       <c r="C21">
-        <v>30.0279870000013</v>
+        <v>29.882386000000501</v>
       </c>
       <c r="D21">
-        <v>81.400444999998996</v>
+        <v>89.852418999998704</v>
       </c>
       <c r="E21">
-        <v>262.18401799999799</v>
+        <v>297.87461099999302</v>
       </c>
       <c r="F21">
-        <v>17.9963039999693</v>
+        <v>21.152612999990101</v>
       </c>
       <c r="G21">
-        <v>37.163927999999103</v>
+        <v>47.126156999999203</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>428.77268199996701</v>
+      </c>
+      <c r="C22">
+        <v>30.0279870000013</v>
+      </c>
+      <c r="D22">
+        <v>81.400444999998996</v>
+      </c>
+      <c r="E22">
+        <v>262.18401799999799</v>
+      </c>
+      <c r="F22">
+        <v>17.9963039999693</v>
+      </c>
+      <c r="G22">
+        <v>37.163927999999103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>515.80502999998498</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>32.979467999999699</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>88.396274999999093</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>326.13471199999202</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>24.640562999994799</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>43.654012000000101</v>
       </c>
     </row>
@@ -5072,11 +5101,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70253BBB-AAC2-7A4A-AA5A-4500351A4D22}">
   <dimension ref="C47:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
@@ -5085,10 +5117,10 @@
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48">
-        <v>1.6125</v>
+        <v>14.898999999999999</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
@@ -5101,29 +5133,32 @@
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <v>14.898999999999999</v>
+        <v>2.1086</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D51">
-        <v>1.0423</v>
+        <v>1.6125</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D52">
-        <v>2.1086</v>
+        <v>1.0423</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="C48:D52">
+    <sortCondition descending="1" ref="D48:D52"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5133,12 +5168,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D7ABBA-C98D-C346-A771-14790F259A85}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Recalc dss_solve detailed timing
</commit_message>
<xml_diff>
--- a/powerflowpy/tests/timings/dss_detailed_timing.xlsx
+++ b/powerflowpy/tests/timings/dss_detailed_timing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elainelaguerta/Dropbox/LBNL/LinDist3Flow/powerflowpy/tests/timings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18272C-A713-454F-BF86-D6A55E91B6D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B889B3-C9D1-BF41-95F6-F821BE7584A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dss_detailed_timing_data" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>total_time</t>
-  </si>
-  <si>
-    <t>final_calcs_time</t>
   </si>
   <si>
     <t>*fill this in by hand based on slope of linear trend line</t>
@@ -36,25 +33,19 @@
     <t>TIMING DATA FOR DSS. INPUT FILE: powerflowpy/tests/06n3ph_rad_unbal/06node_threephase_radial_unbalanced.dss. All timing data in ms.</t>
   </si>
   <si>
-    <t>init_circuit_time</t>
-  </si>
-  <si>
-    <t>save_loads_time</t>
-  </si>
-  <si>
-    <t>reset_loads_total_time</t>
-  </si>
-  <si>
-    <t>run_solvesnap_total_time</t>
-  </si>
-  <si>
-    <t>num_iterations</t>
-  </si>
-  <si>
     <t>Source code filepath: LinDistFlow/powerflowpy/powerflowpy/dss_solve_detailed_timing.py</t>
   </si>
   <si>
     <t>Source code: LinDist3Flow/powerflowpy/dss_timer.py</t>
+  </si>
+  <si>
+    <t>num_trials</t>
+  </si>
+  <si>
+    <t>setup_time</t>
+  </si>
+  <si>
+    <t>solve_time</t>
   </si>
 </sst>
 </file>
@@ -673,517 +664,15 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="7"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>dss_detailed_timing_data!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>reset_loads_total_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent6">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.14569653674384639"/>
-                  <c:y val="9.9303234577692166E-4"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$E$4:$E$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>14.4324469999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>28.6166410000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.101370000000998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55.031578000000302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>71.480816000000502</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>82.957272000002106</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>105.927956000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>140.62099800000101</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>160.90479500000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>195.29794099999501</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>164.91186099999001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>177.45008699999701</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>180.60015900000101</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>191.84692499999599</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>217.59380299999299</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>229.60053099999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>234.242576000009</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>297.87461099999302</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>262.18401799999799</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>326.13471199999202</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-9DCC-F74F-A016-282964A0E918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>dss_detailed_timing_data!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>save_loads_time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent5">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent5">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent5">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="9525" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.15520902188058835"/>
-                  <c:y val="-4.1115957627598709E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$A$4:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>dss_detailed_timing_data!$D$4:$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>4.7895059999999399</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8133059999999599</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.993594000000099</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.418425999999901</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20.7969919999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>24.827808000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32.489599999999797</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>46.055908000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>46.742635000000199</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65.605849000000205</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49.943229999999303</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>49.508581000000397</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>58.072312000000601</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>59.224690000000997</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>68.974967999999507</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>72.330826999999502</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>70.088992999998396</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>89.852418999998704</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>81.400444999998996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>88.396274999999093</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-9DCC-F74F-A016-282964A0E918}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>dss_detailed_timing_data!$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>final_calcs_time</c:v>
+                  <c:v>total_time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1358,69 +847,69 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>dss_detailed_timing_data!$G$4:$G$23</c:f>
+              <c:f>dss_detailed_timing_data!$D$4:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2.2577189999999301</c:v>
+                  <c:v>6.5319310000000401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2084469999998904</c:v>
+                  <c:v>13.1200789999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3967719999998804</c:v>
+                  <c:v>17.456462000000101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.52736300000001</c:v>
+                  <c:v>24.4564330000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.544297</c:v>
+                  <c:v>29.412649999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.674081999999601</c:v>
+                  <c:v>37.226800999999803</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.968339000000299</c:v>
+                  <c:v>40.291951999999498</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.527332000000101</c:v>
+                  <c:v>46.452623000000102</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.638249000000201</c:v>
+                  <c:v>51.568455999999799</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.730349999999898</c:v>
+                  <c:v>59.729462000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.538242000000199</c:v>
+                  <c:v>63.257553999999097</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.500899000000398</c:v>
+                  <c:v>69.322192000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.383750000000799</c:v>
+                  <c:v>95.346307999999993</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.8098660000005</c:v>
+                  <c:v>81.403766999999803</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32.707938999998397</c:v>
+                  <c:v>92.961579999999799</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33.508222000000899</c:v>
+                  <c:v>154.63052200000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.467724000001603</c:v>
+                  <c:v>171.324974999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>47.126156999999203</c:v>
+                  <c:v>171.096744</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>37.163927999999103</c:v>
+                  <c:v>126.442328</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43.654012000000101</c:v>
+                  <c:v>141.82564099999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,15 +922,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="4"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>dss_detailed_timing_data!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>init_circuit_time</c:v>
+                  <c:v>solve_time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1460,21 +949,21 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent5">
                       <a:satMod val="103000"/>
                       <a:lumMod val="102000"/>
                       <a:tint val="94000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="50000">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent5">
                       <a:satMod val="110000"/>
                       <a:lumMod val="100000"/>
                       <a:shade val="100000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent5">
                       <a:lumMod val="99000"/>
                       <a:satMod val="120000"/>
                       <a:shade val="78000"/>
@@ -1485,7 +974,7 @@
               </a:gradFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1496,7 +985,7 @@
             <c:spPr>
               <a:ln w="9525" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1507,8 +996,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14560141189247905"/>
-                  <c:y val="1.4378292641477369E-3"/>
+                  <c:x val="0.15520902188058835"/>
+                  <c:y val="-4.1115957627598709E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1614,64 +1103,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.039534</c:v>
+                  <c:v>5.2067200000001002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9911470000000202</c:v>
+                  <c:v>10.2933629999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.4325089999999099</c:v>
+                  <c:v>13.297072000000201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9425699999999804</c:v>
+                  <c:v>18.328619999999901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4880870000000304</c:v>
+                  <c:v>22.377755999999799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.4209569999999996</c:v>
+                  <c:v>27.720628999999601</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.508993</c:v>
+                  <c:v>30.4574829999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.604229999999699</c:v>
+                  <c:v>35.249998999999697</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.4100939999999</c:v>
+                  <c:v>38.992089999999799</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.569173999999801</c:v>
+                  <c:v>43.445965000000498</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.957875999999999</c:v>
+                  <c:v>47.684900999999499</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.995880000000401</c:v>
+                  <c:v>52.374263999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.676685999999499</c:v>
+                  <c:v>73.143829999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.175610999998799</c:v>
+                  <c:v>61.349631999999701</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.917985999998901</c:v>
+                  <c:v>69.850753000000097</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.7659270000002</c:v>
+                  <c:v>123.459356</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25.994071999999498</c:v>
+                  <c:v>132.28846199999899</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.882386000000501</c:v>
+                  <c:v>138.89283399999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.0279870000013</c:v>
+                  <c:v>97.275656000001206</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32.979467999999699</c:v>
+                  <c:v>108.08937800000101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,20 +1168,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-9DCC-F74F-A016-282964A0E918}"/>
+              <c16:uniqueId val="{00000010-9DCC-F74F-A016-282964A0E918}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="4"/>
+          <c:idx val="5"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>dss_detailed_timing_data!$F$3</c:f>
+              <c:f>dss_detailed_timing_data!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>run_solvesnap_total_time</c:v>
+                  <c:v>setup_time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1711,24 +1200,21 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
+                    <a:schemeClr val="accent6">
                       <a:satMod val="103000"/>
                       <a:lumMod val="102000"/>
                       <a:tint val="94000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
+                    <a:schemeClr val="accent6">
                       <a:satMod val="110000"/>
                       <a:lumMod val="100000"/>
                       <a:shade val="100000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="60000"/>
+                    <a:schemeClr val="accent6">
                       <a:lumMod val="99000"/>
                       <a:satMod val="120000"/>
                       <a:shade val="78000"/>
@@ -1739,9 +1225,7 @@
               </a:gradFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1752,9 +1236,7 @@
             <c:spPr>
               <a:ln w="9525" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1765,8 +1247,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14560141189247905"/>
-                  <c:y val="7.2047810570441285E-3"/>
+                  <c:x val="0.14569653674384639"/>
+                  <c:y val="9.9303234577692166E-4"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1867,69 +1349,69 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>dss_detailed_timing_data!$F$4:$F$23</c:f>
+              <c:f>dss_detailed_timing_data!$B$4:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.95790099999981604</c:v>
+                  <c:v>1.32521099999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0270979999996701</c:v>
+                  <c:v>2.82671599999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8915309999987202</c:v>
+                  <c:v>4.1593899999998696</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8168859999992901</c:v>
+                  <c:v>6.1278130000001996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9829309999986897</c:v>
+                  <c:v>7.0348940000002296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6072669999980196</c:v>
+                  <c:v>9.5061720000002499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9040279999964502</c:v>
+                  <c:v>9.8344689999996202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.616238999997501</c:v>
+                  <c:v>11.2026240000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.9309660000013</c:v>
+                  <c:v>12.576366</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.940408000004801</c:v>
+                  <c:v>16.283497000000501</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.895422000021499</c:v>
+                  <c:v>15.5726529999995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.9488849999943</c:v>
+                  <c:v>16.947928000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.422405999992201</c:v>
+                  <c:v>22.202477999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.019258999984901</c:v>
+                  <c:v>20.054134999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.9980680000041</c:v>
+                  <c:v>23.110826999999698</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.1020319999942</c:v>
+                  <c:v>31.171165999999801</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.7609230000037</c:v>
+                  <c:v>39.0365129999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21.152612999990101</c:v>
+                  <c:v>32.203909999999702</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.9963039999693</c:v>
+                  <c:v>29.166671999999199</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.640562999994799</c:v>
+                  <c:v>33.7362629999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1937,7 +1419,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-9DCC-F74F-A016-282964A0E918}"/>
+              <c16:uniqueId val="{00000011-9DCC-F74F-A016-282964A0E918}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1960,20 +1442,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2024,7 +1492,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2083,6 +1551,19 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2133,7 +1614,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2180,35 +1661,17 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
         <c:idx val="5"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="6"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="7"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="8"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="9"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.78133942531856526"/>
-          <c:y val="0.29795207613436808"/>
-          <c:w val="0.21271527147097097"/>
-          <c:h val="0.2324403784059367"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2375,7 +1838,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -2827,21 +2292,15 @@
             <c:strRef>
               <c:f>dss_subroutines!$C$48:$C$54</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>reset_loads_total_time</c:v>
+                  <c:v>total_time</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>save_loads_time</c:v>
+                  <c:v>solve_time</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>final_calcs_time</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>init_circuit_time</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>run_solvesnap_total_time</c:v>
+                  <c:v>setup_time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2853,19 +2312,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.898999999999999</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4188999999999998</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1086</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.6125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0423</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4177,7 +3630,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -4208,16 +3661,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4593,503 +4046,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>23.4771069999994</v>
+        <v>1.32521099999993</v>
       </c>
       <c r="C4">
-        <v>1.039534</v>
+        <v>5.2067200000001002</v>
       </c>
       <c r="D4">
-        <v>4.7895059999999399</v>
-      </c>
-      <c r="E4">
-        <v>14.4324469999997</v>
-      </c>
-      <c r="F4">
-        <v>0.95790099999981604</v>
-      </c>
-      <c r="G4">
-        <v>2.2577189999999301</v>
+        <v>6.5319310000000401</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>46.656638999999899</v>
+        <v>2.82671599999995</v>
       </c>
       <c r="C5">
-        <v>2.9911470000000202</v>
+        <v>10.2933629999999</v>
       </c>
       <c r="D5">
-        <v>8.8133059999999599</v>
-      </c>
-      <c r="E5">
-        <v>28.6166410000003</v>
-      </c>
-      <c r="F5">
-        <v>2.0270979999996701</v>
-      </c>
-      <c r="G5">
-        <v>4.2084469999998904</v>
+        <v>13.1200789999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>69.815775999999602</v>
+        <v>4.1593899999998696</v>
       </c>
       <c r="C6">
-        <v>4.4325089999999099</v>
+        <v>13.297072000000201</v>
       </c>
       <c r="D6">
-        <v>12.993594000000099</v>
-      </c>
-      <c r="E6">
-        <v>43.101370000000998</v>
-      </c>
-      <c r="F6">
-        <v>2.8915309999987202</v>
-      </c>
-      <c r="G6">
-        <v>6.3967719999998804</v>
+        <v>17.456462000000101</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>90.736822999999603</v>
+        <v>6.1278130000001996</v>
       </c>
       <c r="C7">
-        <v>5.9425699999999804</v>
+        <v>18.328619999999901</v>
       </c>
       <c r="D7">
-        <v>16.418425999999901</v>
-      </c>
-      <c r="E7">
-        <v>55.031578000000302</v>
-      </c>
-      <c r="F7">
-        <v>3.8168859999992901</v>
-      </c>
-      <c r="G7">
-        <v>9.52736300000001</v>
+        <v>24.4564330000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>115.293122999999</v>
+        <v>7.0348940000002296</v>
       </c>
       <c r="C8">
-        <v>7.4880870000000304</v>
+        <v>22.377755999999799</v>
       </c>
       <c r="D8">
-        <v>20.7969919999999</v>
-      </c>
-      <c r="E8">
-        <v>71.480816000000502</v>
-      </c>
-      <c r="F8">
-        <v>4.9829309999986897</v>
-      </c>
-      <c r="G8">
-        <v>10.544297</v>
+        <v>29.412649999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>135.48738599999899</v>
+        <v>9.5061720000002499</v>
       </c>
       <c r="C9">
-        <v>9.4209569999999996</v>
+        <v>27.720628999999601</v>
       </c>
       <c r="D9">
-        <v>24.827808000000001</v>
-      </c>
-      <c r="E9">
-        <v>82.957272000002106</v>
-      </c>
-      <c r="F9">
-        <v>5.6072669999980196</v>
-      </c>
-      <c r="G9">
-        <v>12.674081999999601</v>
+        <v>37.226800999999803</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10">
-        <v>174.798915999998</v>
+        <v>9.8344689999996202</v>
       </c>
       <c r="C10">
-        <v>11.508993</v>
+        <v>30.4574829999999</v>
       </c>
       <c r="D10">
-        <v>32.489599999999797</v>
-      </c>
-      <c r="E10">
-        <v>105.927956000001</v>
-      </c>
-      <c r="F10">
-        <v>7.9040279999964502</v>
-      </c>
-      <c r="G10">
-        <v>16.968339000000299</v>
+        <v>40.291951999999498</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11">
-        <v>234.42470699999899</v>
+        <v>11.2026240000004</v>
       </c>
       <c r="C11">
-        <v>14.604229999999699</v>
+        <v>35.249998999999697</v>
       </c>
       <c r="D11">
-        <v>46.055908000000002</v>
-      </c>
-      <c r="E11">
-        <v>140.62099800000101</v>
-      </c>
-      <c r="F11">
-        <v>10.616238999997501</v>
-      </c>
-      <c r="G11">
-        <v>22.527332000000101</v>
+        <v>46.452623000000102</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12">
-        <v>262.62673900000198</v>
+        <v>12.576366</v>
       </c>
       <c r="C12">
-        <v>15.4100939999999</v>
+        <v>38.992089999999799</v>
       </c>
       <c r="D12">
-        <v>46.742635000000199</v>
-      </c>
-      <c r="E12">
-        <v>160.90479500000001</v>
-      </c>
-      <c r="F12">
-        <v>15.9309660000013</v>
-      </c>
-      <c r="G12">
-        <v>23.638249000000201</v>
+        <v>51.568455999999799</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13">
-        <v>334.14372200000003</v>
+        <v>16.283497000000501</v>
       </c>
       <c r="C13">
-        <v>22.569173999999801</v>
+        <v>43.445965000000498</v>
       </c>
       <c r="D13">
-        <v>65.605849000000205</v>
-      </c>
-      <c r="E13">
-        <v>195.29794099999501</v>
-      </c>
-      <c r="F13">
-        <v>18.940408000004801</v>
-      </c>
-      <c r="G13">
-        <v>31.730349999999898</v>
+        <v>59.729462000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14">
-        <v>269.24663100001197</v>
+        <v>15.5726529999995</v>
       </c>
       <c r="C14">
-        <v>17.957875999999999</v>
+        <v>47.684900999999499</v>
       </c>
       <c r="D14">
-        <v>49.943229999999303</v>
-      </c>
-      <c r="E14">
-        <v>164.91186099999001</v>
-      </c>
-      <c r="F14">
-        <v>11.895422000021499</v>
-      </c>
-      <c r="G14">
-        <v>24.538242000000199</v>
+        <v>63.257553999999097</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15">
-        <v>290.40433199999302</v>
+        <v>16.947928000000001</v>
       </c>
       <c r="C15">
-        <v>21.995880000000401</v>
+        <v>52.374263999999997</v>
       </c>
       <c r="D15">
-        <v>49.508581000000397</v>
-      </c>
-      <c r="E15">
-        <v>177.45008699999701</v>
-      </c>
-      <c r="F15">
-        <v>12.9488849999943</v>
-      </c>
-      <c r="G15">
-        <v>28.500899000000398</v>
+        <v>69.322192000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16">
-        <v>297.15531299999401</v>
+        <v>22.202477999999999</v>
       </c>
       <c r="C16">
-        <v>19.676685999999499</v>
+        <v>73.143829999999994</v>
       </c>
       <c r="D16">
-        <v>58.072312000000601</v>
-      </c>
-      <c r="E16">
-        <v>180.60015900000101</v>
-      </c>
-      <c r="F16">
-        <v>12.422405999992201</v>
-      </c>
-      <c r="G16">
-        <v>26.383750000000799</v>
+        <v>95.346307999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17">
-        <v>314.076350999981</v>
+        <v>20.054134999999999</v>
       </c>
       <c r="C17">
-        <v>22.175610999998799</v>
+        <v>61.349631999999701</v>
       </c>
       <c r="D17">
-        <v>59.224690000000997</v>
-      </c>
-      <c r="E17">
-        <v>191.84692499999599</v>
-      </c>
-      <c r="F17">
-        <v>13.019258999984901</v>
-      </c>
-      <c r="G17">
-        <v>27.8098660000005</v>
+        <v>81.403766999999803</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18">
-        <v>358.19276399999399</v>
+        <v>23.110826999999698</v>
       </c>
       <c r="C18">
-        <v>23.917985999998901</v>
+        <v>69.850753000000097</v>
       </c>
       <c r="D18">
-        <v>68.974967999999507</v>
-      </c>
-      <c r="E18">
-        <v>217.59380299999299</v>
-      </c>
-      <c r="F18">
-        <v>14.9980680000041</v>
-      </c>
-      <c r="G18">
-        <v>32.707938999998397</v>
+        <v>92.961579999999799</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19">
-        <v>376.30753899999502</v>
+        <v>31.171165999999801</v>
       </c>
       <c r="C19">
-        <v>24.7659270000002</v>
+        <v>123.459356</v>
       </c>
       <c r="D19">
-        <v>72.330826999999502</v>
-      </c>
-      <c r="E19">
-        <v>229.60053099999999</v>
-      </c>
-      <c r="F19">
-        <v>16.1020319999942</v>
-      </c>
-      <c r="G19">
-        <v>33.508222000000899</v>
+        <v>154.63052200000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20">
-        <v>379.55428800001198</v>
+        <v>39.0365129999998</v>
       </c>
       <c r="C20">
-        <v>25.994071999999498</v>
+        <v>132.28846199999899</v>
       </c>
       <c r="D20">
-        <v>70.088992999998396</v>
-      </c>
-      <c r="E20">
-        <v>234.242576000009</v>
-      </c>
-      <c r="F20">
-        <v>15.7609230000037</v>
-      </c>
-      <c r="G20">
-        <v>33.467724000001603</v>
+        <v>171.324974999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21">
-        <v>485.88818599998098</v>
+        <v>32.203909999999702</v>
       </c>
       <c r="C21">
-        <v>29.882386000000501</v>
+        <v>138.89283399999999</v>
       </c>
       <c r="D21">
-        <v>89.852418999998704</v>
-      </c>
-      <c r="E21">
-        <v>297.87461099999302</v>
-      </c>
-      <c r="F21">
-        <v>21.152612999990101</v>
-      </c>
-      <c r="G21">
-        <v>47.126156999999203</v>
+        <v>171.096744</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22">
-        <v>428.77268199996701</v>
+        <v>29.166671999999199</v>
       </c>
       <c r="C22">
-        <v>30.0279870000013</v>
+        <v>97.275656000001206</v>
       </c>
       <c r="D22">
-        <v>81.400444999998996</v>
-      </c>
-      <c r="E22">
-        <v>262.18401799999799</v>
-      </c>
-      <c r="F22">
-        <v>17.9963039999693</v>
-      </c>
-      <c r="G22">
-        <v>37.163927999999103</v>
+        <v>126.442328</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23">
-        <v>515.80502999998498</v>
+        <v>33.7362629999988</v>
       </c>
       <c r="C23">
-        <v>32.979467999999699</v>
+        <v>108.08937800000101</v>
       </c>
       <c r="D23">
-        <v>88.396274999999093</v>
-      </c>
-      <c r="E23">
-        <v>326.13471199999202</v>
-      </c>
-      <c r="F23">
-        <v>24.640562999994799</v>
-      </c>
-      <c r="G23">
-        <v>43.654012000000101</v>
+        <v>141.82564099999999</v>
       </c>
     </row>
   </sheetData>
@@ -5099,10 +4365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70253BBB-AAC2-7A4A-AA5A-4500351A4D22}">
-  <dimension ref="C47:D52"/>
+  <dimension ref="C47:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5112,47 +4378,31 @@
   <sheetData>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>14.898999999999999</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>4.4188999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>2.1086</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51">
-        <v>1.6125</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52">
-        <v>1.0423</v>
+        <v>1.8</v>
       </c>
     </row>
   </sheetData>
@@ -5176,7 +4426,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>